<commit_message>
This file are uploaded for v2 enhancemment
</commit_message>
<xml_diff>
--- a/queries.xlsx
+++ b/queries.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -22,40 +22,30 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t xml:space="preserve">USE my_database;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CREATE TABLE table1 (
-    id INT AUTO_INCREMENT PRIMARY KEY,
-    name VARCHAR(50) NOT NULL
-);
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CREATE TABLE table2 (
-    id INT AUTO_INCREMENT PRIMARY KEY,
-    table1_id INT NOT NULL,
-    value INT NOT NULL,
-    FOREIGN KEY (table1_id) REFERENCES table1(id)
-);
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSERT INTO table1 (name) VALUES
-    ('John'),
-    ('Sarah'),
-    ('Peter'),
-    ('Mary'),
-    ('Tom');
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INSERT INTO table2 (table1_id, value) VALUES
-    (1, 10),
-    (1, 20),
-    (2, 30),
-    (2, 40),
-    (3, 50);
+    <t xml:space="preserve">SELECT * FROM table1;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT name FROM table1 WHERE id &gt; 2;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT id, value FROM table2 WHERE value &lt;= 40;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT t1.id, t1.name, t2.value 
+FROM table1 AS t1 
+JOIN table2 AS t2 
+ON t1.id = t2.table1_id;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT t1.name, AVG(t2.value) 
+FROM table1 AS t1 
+JOIN table2 AS t2 
+ON t1.id = t2.table1_id 
+GROUP BY t1.name;
 </t>
   </si>
 </sst>
@@ -71,6 +61,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -89,8 +80,8 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val=""/>
-      <family val="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -136,12 +127,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -164,34 +163,37 @@
   </sheetPr>
   <dimension ref="A2:A11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="5" customFormat="false" ht="67.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="93.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="107.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="93.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+    <row r="9" customFormat="false" ht="186.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="93.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+    <row r="11" customFormat="false" ht="226.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>